<commit_message>
fixes in the code.
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pCloudFolder\Repositories\Databaseroject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E373416-05F1-4AEE-8B25-EFC74714625D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096A369A-EE1D-45CF-ACDA-5B496070055A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{72310E18-2CB3-4089-87E6-D1772337C237}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>I.</t>
   </si>
@@ -189,10 +189,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>SS_category
-SS_Advertisement</t>
   </si>
   <si>
     <t>SS_category
@@ -224,10 +220,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -253,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -267,11 +269,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4672CCAB-24F9-4FAB-B7BC-D26AC2FAFA0A}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -710,6 +730,9 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="C6" s="12" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -722,20 +745,20 @@
         <v>46</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="C8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -744,9 +767,11 @@
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -756,7 +781,9 @@
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -767,10 +794,10 @@
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -781,10 +808,10 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -804,7 +831,9 @@
       <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -814,7 +843,9 @@
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -824,7 +855,7 @@
       <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D16" s="2"/>
@@ -842,35 +873,37 @@
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="2"/>
+      <c r="C18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -880,7 +913,9 @@
       <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -945,8 +980,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>